<commit_message>
update big genes BOM
</commit_message>
<xml_diff>
--- a/docs/big_genes/ksoloti_big_genes_bom.xlsx
+++ b/docs/big_genes/ksoloti_big_genes_bom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="98">
   <si>
     <t xml:space="preserve">Ref</t>
   </si>
@@ -209,16 +209,68 @@
   </si>
   <si>
     <t xml:space="preserve">RED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED3, LED4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED_Dual_AKA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED_D3.0mm-3_marked + 4mm standoff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED5, LED6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED_SMD:LED_0805_2012Metric_Pad1.15x1.40mm_HandSolder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optional 0805 LEDs as gate indicators, can also solder a generic 3mm through hole LED to the SMD pads (at least that’s what I’ve been doing)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adafruit_PDM_microphone_breakout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adafruit PDM microphone breakout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">optional, at discretion of builder
+https://learn.adafruit.com/adafruit-pdm-microphone-breakout/overview</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OLED1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">128x64_OLED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">128x64OLED_1_3in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RV1, RV2, RV3, RV4, RV5, RV6, RV7, RV8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B10k to B50k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALPS_POT_VERTICAL_PS</t>
   </si>
   <si>
     <r>
       <rPr>
+        <b val="true"/>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">LED_D3.0mm_marked</t>
+      <t xml:space="preserve">B50k recommended, different</t>
     </r>
     <r>
       <rPr>
@@ -226,24 +278,16 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> + 4mm standoff</t>
+      <t xml:space="preserve"> from</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">LED3, LED4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LED_Dual_AKA</t>
-  </si>
-  <si>
     <r>
       <rPr>
+        <b val="true"/>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">LED_D3.0mm-3_marked</t>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -251,79 +295,8 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> + 4mm standoff</t>
+      <t xml:space="preserve">Gills (same part as Gills except resistance value)</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">LED5, LED6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LED_SMD:LED_0805_2012Metric_Pad1.15x1.40mm_HandSolder</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF808080"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Optional 0805 LEDs as g</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF808080"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">ate indicators</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF808080"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">, can also solder a generic 3mm through hole LED to the SMD pads (at least that’s what I’ve been doing)</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">M1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adafruit_PDM_microphone_breakout</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adafruit PDM microphone breakout</t>
-  </si>
-  <si>
-    <t xml:space="preserve">optional, at discretion of builder
-https://learn.adafruit.com/adafruit-pdm-microphone-breakout/overview</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OLED1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">128x64_OLED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">128x64OLED_1_3in</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RV1, RV2, RV3, RV4, RV5, RV6, RV7, RV8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B10k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALPS_POT_VERTICAL_PS</t>
   </si>
   <si>
     <t xml:space="preserve">SW1, SW2</t>
@@ -399,59 +372,6 @@
     <t xml:space="preserve">10k</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Trimmer Potentiometer</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">different</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> from</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Gills</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">M3 6mm screw</t>
   </si>
   <si>
@@ -483,7 +403,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -520,18 +440,12 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -592,7 +506,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -629,7 +543,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -728,9 +646,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>4130640</xdr:colOff>
+      <xdr:colOff>4130280</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>31680</xdr:rowOff>
+      <xdr:rowOff>31320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -744,7 +662,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6896880" y="8138160"/>
-          <a:ext cx="4130640" cy="4130640"/>
+          <a:ext cx="4130280" cy="4130280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -872,8 +790,8 @@
   </sheetPr>
   <dimension ref="A1:XFD42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="31.109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1191,7 +1109,7 @@
         <v>62</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>60</v>
@@ -1200,16 +1118,16 @@
     </row>
     <row r="18" s="7" customFormat="true" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B18" s="4" t="n">
         <v>2</v>
       </c>
       <c r="C18" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>65</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>66</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>60</v>
@@ -1219,53 +1137,53 @@
     </row>
     <row r="19" s="7" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B19" s="6" t="n">
         <v>2</v>
       </c>
       <c r="C19" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="E19" s="6" t="s">
         <v>69</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>70</v>
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="3"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B20" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C20" s="6" t="s">
+      <c r="D20" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="E20" s="8" t="s">
         <v>73</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>74</v>
       </c>
       <c r="F20" s="6"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B21" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C21" s="4" t="s">
+      <c r="D21" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>77</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>15</v>
@@ -1274,19 +1192,19 @@
     </row>
     <row r="22" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B22" s="4" t="n">
         <v>8</v>
       </c>
       <c r="C22" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="E22" s="9" t="s">
         <v>80</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="F22" s="4"/>
     </row>
@@ -1341,7 +1259,7 @@
         <v>86</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F25" s="4"/>
     </row>
@@ -1351,11 +1269,11 @@
         <v>4</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F26" s="4"/>
     </row>
@@ -1365,56 +1283,56 @@
         <v>4</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5"/>
       <c r="B28" s="5" t="n">
         <v>1</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F28" s="5"/>
-      <c r="G28" s="9"/>
-      <c r="XFD28" s="9"/>
-    </row>
-    <row r="29" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G28" s="10"/>
+      <c r="XFD28" s="10"/>
+    </row>
+    <row r="29" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5"/>
       <c r="B29" s="5" t="n">
         <v>1</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F29" s="5"/>
+      <c r="G29" s="10"/>
+    </row>
+    <row r="30" customFormat="false" ht="194.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="12"/>
+      <c r="B30" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F29" s="5"/>
-      <c r="G29" s="9"/>
-    </row>
-    <row r="30" customFormat="false" ht="194.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="11"/>
-      <c r="B30" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="D30" s="11"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="11"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="12"/>
     </row>
     <row r="42" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1"/>

</xml_diff>